<commit_message>
Fin de la Phase 1
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Planification.xlsx
+++ b/C61/Phase 1/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\C61-ProjetSynthese\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E708AF07-7A6E-48A7-8718-8259C48EB4EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34834CA-1EC4-4CFD-97C7-549CD0C1F2DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,6 +44,20 @@
     <author>tc={81C60AC0-D935-46DE-84D8-EC6328CEDC30}</author>
     <author>tc={85ED4ADB-3F6C-4847-A56B-1292A1C6C7C2}</author>
     <author>tc={623676B3-14AA-4184-9428-55ADD2304DA4}</author>
+    <author>tc={1DC6ABEE-7B3E-4A9F-B9F6-F46BC688CCE7}</author>
+    <author>tc={2852775C-1FBD-44C4-BAC1-A431D0981B5F}</author>
+    <author>tc={FD1A719F-3BCD-43EA-9D4D-18DEB5B2F5B0}</author>
+    <author>tc={81164D7C-C2FB-4244-8414-CC41969DF381}</author>
+    <author>tc={5395E750-0FFD-4E03-80CD-6069BBA6BD3D}</author>
+    <author>tc={8273DA2D-5529-4100-9525-4612A9DD7ED1}</author>
+    <author>tc={CF6E1DF2-5610-47EB-B066-EC977CD7FA91}</author>
+    <author>tc={74B595E4-52D0-481A-B607-E17032472E4B}</author>
+    <author>tc={A6648092-3E5F-4913-8427-45C9B466D863}</author>
+    <author>tc={9B43A026-F2D0-4C8C-9703-B31060206748}</author>
+    <author>tc={C1705974-8169-4660-B0F6-44A9345D0878}</author>
+    <author>tc={3E9CB20E-C6B4-4C89-B285-CAB63B422B3F}</author>
+    <author>tc={BD812E72-99A0-464D-95E6-D06ACD7A7C9C}</author>
+    <author>tc={5E04ADCF-5B9E-413B-8541-DDB20D8F2750}</author>
   </authors>
   <commentList>
     <comment ref="D8" authorId="0" shapeId="0" xr:uid="{9F0570D1-CBA7-43A1-9070-AFCA2B0D67C9}">
@@ -78,6 +92,118 @@
     facile, moyen, difficile, incertain</t>
       </text>
     </comment>
+    <comment ref="C9" authorId="4" shapeId="0" xr:uid="{1DC6ABEE-7B3E-4A9F-B9F6-F46BC688CCE7}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Affichage incluant toujours : Incluant CSS, JS et html</t>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="5" shapeId="0" xr:uid="{2852775C-1FBD-44C4-BAC1-A431D0981B5F}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Création des setters pour la BD</t>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="6" shapeId="0" xr:uid="{FD1A719F-3BCD-43EA-9D4D-18DEB5B2F5B0}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    gestion de l'authentification dans cette étape</t>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="7" shapeId="0" xr:uid="{81164D7C-C2FB-4244-8414-CC41969DF381}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    gestion des formulaires et affichage des erreurs le cas échéant</t>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="8" shapeId="0" xr:uid="{5395E750-0FFD-4E03-80CD-6069BBA6BD3D}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    écriture dans la BD</t>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="9" shapeId="0" xr:uid="{8273DA2D-5529-4100-9525-4612A9DD7ED1}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    doit lire dans BD évènement pour afficher les évènements en lien avec le userID</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="10" shapeId="0" xr:uid="{CF6E1DF2-5610-47EB-B066-EC977CD7FA91}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    et création d'une disponibilité pour le créateur</t>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="11" shapeId="0" xr:uid="{74B595E4-52D0-481A-B607-E17032472E4B}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Redirection vers acceuil si client non authentifié essaie d'accéder à une page</t>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="12" shapeId="0" xr:uid="{A6648092-3E5F-4913-8427-45C9B466D863}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Initialisation des paramètres : nb de genérations maximales, case horaire de l'évènement et les disponibilités des participants</t>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="13" shapeId="0" xr:uid="{9B43A026-F2D0-4C8C-9703-B31060206748}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Ne doit pas avoir de lien vers le problème directement.</t>
+      </text>
+    </comment>
+    <comment ref="C38" authorId="14" shapeId="0" xr:uid="{C1705974-8169-4660-B0F6-44A9345D0878}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Un seul choix pour la disponibilité. Réserve automatiquement la plage horaire. La plage devient indisponible pour les autres usagers.</t>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="15" shapeId="0" xr:uid="{3E9CB20E-C6B4-4C89-B285-CAB63B422B3F}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Possibilité d'ajouter une préférence. Doit être tenu en compte comme une variable par le ScheduleOptimizer</t>
+      </text>
+    </comment>
+    <comment ref="C44" authorId="16" shapeId="0" xr:uid="{BD812E72-99A0-464D-95E6-D06ACD7A7C9C}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Envoyer un JSON avec les données à être affichée pour l'affichage. ET pour le calcul du script algoGen</t>
+      </text>
+    </comment>
+    <comment ref="C52" authorId="17" shapeId="0" xr:uid="{5E04ADCF-5B9E-413B-8541-DDB20D8F2750}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Fonctionnalité similaire à Doodle. Un sondage seulement.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -105,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
   <si>
     <t>Dany Viens</t>
   </si>
@@ -342,13 +468,22 @@
   </si>
   <si>
     <t>20, 22</t>
+  </si>
+  <si>
+    <t>1,4,8,11,18,34</t>
+  </si>
+  <si>
+    <t>34, 18, 15, 11, 7, 4, 1</t>
+  </si>
+  <si>
+    <t>12, 35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +498,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -901,6 +1042,48 @@
   <threadedComment ref="G8" dT="2021-02-26T05:17:12.92" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{623676B3-14AA-4184-9428-55ADD2304DA4}">
     <text>facile, moyen, difficile, incertain</text>
   </threadedComment>
+  <threadedComment ref="C9" dT="2021-03-04T01:57:39.57" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{1DC6ABEE-7B3E-4A9F-B9F6-F46BC688CCE7}">
+    <text>Affichage incluant toujours : Incluant CSS, JS et html</text>
+  </threadedComment>
+  <threadedComment ref="C10" dT="2021-03-04T01:58:02.23" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{2852775C-1FBD-44C4-BAC1-A431D0981B5F}">
+    <text>Création des setters pour la BD</text>
+  </threadedComment>
+  <threadedComment ref="C11" dT="2021-03-04T01:58:31.14" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{FD1A719F-3BCD-43EA-9D4D-18DEB5B2F5B0}">
+    <text>gestion de l'authentification dans cette étape</text>
+  </threadedComment>
+  <threadedComment ref="C14" dT="2021-03-04T01:58:57.09" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{81164D7C-C2FB-4244-8414-CC41969DF381}">
+    <text>gestion des formulaires et affichage des erreurs le cas échéant</text>
+  </threadedComment>
+  <threadedComment ref="C15" dT="2021-03-04T01:59:11.18" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{5395E750-0FFD-4E03-80CD-6069BBA6BD3D}">
+    <text>écriture dans la BD</text>
+  </threadedComment>
+  <threadedComment ref="C17" dT="2021-03-04T01:59:38.54" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{8273DA2D-5529-4100-9525-4612A9DD7ED1}">
+    <text>doit lire dans BD évènement pour afficher les évènements en lien avec le userID</text>
+  </threadedComment>
+  <threadedComment ref="C20" dT="2021-03-04T01:59:57.71" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{CF6E1DF2-5610-47EB-B066-EC977CD7FA91}">
+    <text>et création d'une disponibilité pour le créateur</text>
+  </threadedComment>
+  <threadedComment ref="C24" dT="2021-03-04T02:00:37.21" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{74B595E4-52D0-481A-B607-E17032472E4B}">
+    <text>Redirection vers acceuil si client non authentifié essaie d'accéder à une page</text>
+  </threadedComment>
+  <threadedComment ref="C28" dT="2021-03-04T02:01:47.43" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{A6648092-3E5F-4913-8427-45C9B466D863}">
+    <text>Initialisation des paramètres : nb de genérations maximales, case horaire de l'évènement et les disponibilités des participants</text>
+  </threadedComment>
+  <threadedComment ref="C30" dT="2021-03-04T02:02:08.42" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{9B43A026-F2D0-4C8C-9703-B31060206748}">
+    <text>Ne doit pas avoir de lien vers le problème directement.</text>
+  </threadedComment>
+  <threadedComment ref="C38" dT="2021-03-04T02:04:06.55" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{C1705974-8169-4660-B0F6-44A9345D0878}">
+    <text>Un seul choix pour la disponibilité. Réserve automatiquement la plage horaire. La plage devient indisponible pour les autres usagers.</text>
+  </threadedComment>
+  <threadedComment ref="C39" dT="2021-03-04T02:04:37.30" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{3E9CB20E-C6B4-4C89-B285-CAB63B422B3F}">
+    <text>Possibilité d'ajouter une préférence. Doit être tenu en compte comme une variable par le ScheduleOptimizer</text>
+  </threadedComment>
+  <threadedComment ref="C44" dT="2021-03-04T02:05:22.67" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{BD812E72-99A0-464D-95E6-D06ACD7A7C9C}">
+    <text>Envoyer un JSON avec les données à être affichée pour l'affichage. ET pour le calcul du script algoGen</text>
+  </threadedComment>
+  <threadedComment ref="C52" dT="2021-03-04T02:05:57.87" personId="{062A69FF-1505-4449-A6A7-1A51CCE61D02}" id="{5E04ADCF-5B9E-413B-8541-DDB20D8F2750}">
+    <text>Fonctionnalité similaire à Doodle. Un sondage seulement.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -908,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="21">
-        <f>IF(G9="facile",1,IF(G9="moyen",5,IF(G9="difficile",10,7.5)))</f>
+        <f t="shared" ref="H9:H14" si="0">IF(G9="facile",1,IF(G9="moyen",5,IF(G9="difficile",10,7.5)))</f>
         <v>1</v>
       </c>
       <c r="I9" s="21">
@@ -1011,7 +1194,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="21">
-        <f>IF(G10="facile",1,IF(G10="moyen",5,IF(G10="difficile",10,7.5)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I10" s="21">
@@ -1038,7 +1221,7 @@
         <v>12</v>
       </c>
       <c r="H11" s="21">
-        <f>IF(G11="facile",1,IF(G11="moyen",5,IF(G11="difficile",10,7.5)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I11" s="21">
@@ -1065,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="21">
-        <f>IF(G12="facile",1,IF(G12="moyen",5,IF(G12="difficile",10,7.5)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I12" s="21">
@@ -1092,7 +1275,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="21">
-        <f>IF(G13="facile",1,IF(G13="moyen",5,IF(G13="difficile",10,7.5)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I13" s="21">
@@ -1119,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="21">
-        <f>IF(G14="facile",1,IF(G14="moyen",5,IF(G14="difficile",10,7.5)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I14" s="21">
@@ -1173,7 +1356,7 @@
         <v>12</v>
       </c>
       <c r="H16" s="21">
-        <f>IF(G16="facile",1,IF(G16="moyen",5,IF(G16="difficile",10,7.5)))</f>
+        <f t="shared" ref="H16:H53" si="1">IF(G16="facile",1,IF(G16="moyen",5,IF(G16="difficile",10,7.5)))</f>
         <v>5</v>
       </c>
       <c r="I16" s="21">
@@ -1200,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="H17" s="21">
-        <f>IF(G17="facile",1,IF(G17="moyen",5,IF(G17="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I17" s="21">
@@ -1227,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="21">
-        <f>IF(G18="facile",1,IF(G18="moyen",5,IF(G18="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I18" s="21">
@@ -1254,7 +1437,7 @@
         <v>12</v>
       </c>
       <c r="H19" s="21">
-        <f>IF(G19="facile",1,IF(G19="moyen",5,IF(G19="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I19" s="21">
@@ -1281,7 +1464,7 @@
         <v>43</v>
       </c>
       <c r="H20" s="21">
-        <f>IF(G20="facile",1,IF(G20="moyen",5,IF(G20="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I20" s="21">
@@ -1308,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="21">
-        <f>IF(G21="facile",1,IF(G21="moyen",5,IF(G21="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I21" s="21">
@@ -1335,7 +1518,7 @@
         <v>12</v>
       </c>
       <c r="H22" s="21">
-        <f>IF(G22="facile",1,IF(G22="moyen",5,IF(G22="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I22" s="21">
@@ -1362,7 +1545,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="21">
-        <f>IF(G23="facile",1,IF(G23="moyen",5,IF(G23="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I23" s="21">
@@ -1389,7 +1572,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="4">
-        <f>IF(G24="facile",1,IF(G24="moyen",5,IF(G24="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I24" s="4">
@@ -1416,7 +1599,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="4">
-        <f>IF(G25="facile",1,IF(G25="moyen",5,IF(G25="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I25" s="4">
@@ -1443,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="H26" s="4">
-        <f>IF(G26="facile",1,IF(G26="moyen",5,IF(G26="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I26" s="4">
@@ -1470,7 +1653,7 @@
         <v>43</v>
       </c>
       <c r="H27" s="4">
-        <f>IF(G27="facile",1,IF(G27="moyen",5,IF(G27="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I27" s="4">
@@ -1497,7 +1680,7 @@
         <v>11</v>
       </c>
       <c r="H28" s="4">
-        <f>IF(G28="facile",1,IF(G28="moyen",5,IF(G28="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I28" s="4">
@@ -1524,7 +1707,7 @@
         <v>43</v>
       </c>
       <c r="H29" s="4">
-        <f>IF(G29="facile",1,IF(G29="moyen",5,IF(G29="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I29" s="4">
@@ -1551,7 +1734,7 @@
         <v>43</v>
       </c>
       <c r="H30" s="4">
-        <f>IF(G30="facile",1,IF(G30="moyen",5,IF(G30="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I30" s="4">
@@ -1578,7 +1761,7 @@
         <v>12</v>
       </c>
       <c r="H31" s="4">
-        <f>IF(G31="facile",1,IF(G31="moyen",5,IF(G31="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I31" s="4">
@@ -1605,7 +1788,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="4">
-        <f>IF(G32="facile",1,IF(G32="moyen",5,IF(G32="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I32" s="4">
@@ -1632,7 +1815,7 @@
         <v>12</v>
       </c>
       <c r="H33" s="4">
-        <f>IF(G33="facile",1,IF(G33="moyen",5,IF(G33="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I33" s="4">
@@ -1659,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="H34" s="4">
-        <f>IF(G34="facile",1,IF(G34="moyen",5,IF(G34="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I34" s="4">
@@ -1686,7 +1869,7 @@
         <v>10</v>
       </c>
       <c r="H35" s="4">
-        <f>IF(G35="facile",1,IF(G35="moyen",5,IF(G35="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I35" s="4">
@@ -1713,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="H36" s="4">
-        <f>IF(G36="facile",1,IF(G36="moyen",5,IF(G36="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I36" s="4">
@@ -1740,7 +1923,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="4">
-        <f>IF(G37="facile",1,IF(G37="moyen",5,IF(G37="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I37" s="4">
@@ -1767,7 +1950,7 @@
         <v>12</v>
       </c>
       <c r="H38" s="4">
-        <f>IF(G38="facile",1,IF(G38="moyen",5,IF(G38="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I38" s="4">
@@ -1794,7 +1977,7 @@
         <v>43</v>
       </c>
       <c r="H39" s="4">
-        <f>IF(G39="facile",1,IF(G39="moyen",5,IF(G39="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I39" s="4">
@@ -1811,7 +1994,9 @@
       <c r="D40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2">
+        <v>34.35</v>
+      </c>
       <c r="F40" s="2" t="s">
         <v>23</v>
       </c>
@@ -1819,7 +2004,7 @@
         <v>43</v>
       </c>
       <c r="H40" s="2">
-        <f>IF(G40="facile",1,IF(G40="moyen",5,IF(G40="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I40" s="2">
@@ -1836,7 +2021,9 @@
       <c r="D41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2">
+        <v>32</v>
+      </c>
       <c r="F41" s="2" t="s">
         <v>23</v>
       </c>
@@ -1844,7 +2031,7 @@
         <v>12</v>
       </c>
       <c r="H41" s="2">
-        <f>IF(G41="facile",1,IF(G41="moyen",5,IF(G41="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I41" s="2">
@@ -1861,7 +2048,9 @@
       <c r="D42" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="2"/>
+      <c r="E42" s="2">
+        <v>33</v>
+      </c>
       <c r="F42" s="2" t="s">
         <v>23</v>
       </c>
@@ -1869,7 +2058,7 @@
         <v>12</v>
       </c>
       <c r="H42" s="2">
-        <f>IF(G42="facile",1,IF(G42="moyen",5,IF(G42="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I42" s="2">
@@ -1894,7 +2083,7 @@
         <v>43</v>
       </c>
       <c r="H43" s="2">
-        <f>IF(G43="facile",1,IF(G43="moyen",5,IF(G43="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I43" s="2">
@@ -1921,7 +2110,7 @@
         <v>11</v>
       </c>
       <c r="H44" s="2">
-        <f>IF(G44="facile",1,IF(G44="moyen",5,IF(G44="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I44" s="2">
@@ -1938,7 +2127,9 @@
       <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="F45" s="2" t="s">
         <v>24</v>
       </c>
@@ -1946,7 +2137,7 @@
         <v>12</v>
       </c>
       <c r="H45" s="2">
-        <f>IF(G45="facile",1,IF(G45="moyen",5,IF(G45="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I45" s="2">
@@ -1963,7 +2154,9 @@
       <c r="D46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1971,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="H46" s="2">
-        <f>IF(G46="facile",1,IF(G46="moyen",5,IF(G46="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I46" s="2">
@@ -1988,7 +2181,9 @@
       <c r="D47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2">
+        <v>21</v>
+      </c>
       <c r="F47" s="2" t="s">
         <v>24</v>
       </c>
@@ -1996,7 +2191,7 @@
         <v>11</v>
       </c>
       <c r="H47" s="2">
-        <f>IF(G47="facile",1,IF(G47="moyen",5,IF(G47="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I47" s="2">
@@ -2013,7 +2208,9 @@
       <c r="D48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2">
+        <v>21</v>
+      </c>
       <c r="F48" s="2" t="s">
         <v>24</v>
       </c>
@@ -2021,7 +2218,7 @@
         <v>11</v>
       </c>
       <c r="H48" s="2">
-        <f>IF(G48="facile",1,IF(G48="moyen",5,IF(G48="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I48" s="2">
@@ -2038,7 +2235,9 @@
       <c r="D49" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2">
+        <v>21</v>
+      </c>
       <c r="F49" s="2" t="s">
         <v>24</v>
       </c>
@@ -2046,7 +2245,7 @@
         <v>11</v>
       </c>
       <c r="H49" s="2">
-        <f>IF(G49="facile",1,IF(G49="moyen",5,IF(G49="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I49" s="2">
@@ -2063,7 +2262,9 @@
       <c r="D50" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2">
+        <v>32.33</v>
+      </c>
       <c r="F50" s="2" t="s">
         <v>42</v>
       </c>
@@ -2071,7 +2272,7 @@
         <v>43</v>
       </c>
       <c r="H50" s="2">
-        <f>IF(G50="facile",1,IF(G50="moyen",5,IF(G50="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I50" s="2">
@@ -2088,7 +2289,9 @@
       <c r="D51" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F51" s="2" t="s">
         <v>42</v>
       </c>
@@ -2096,7 +2299,7 @@
         <v>12</v>
       </c>
       <c r="H51" s="2">
-        <f>IF(G51="facile",1,IF(G51="moyen",5,IF(G51="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I51" s="2">
@@ -2113,7 +2316,9 @@
       <c r="D52" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F52" s="2" t="s">
         <v>42</v>
       </c>
@@ -2121,7 +2326,7 @@
         <v>12</v>
       </c>
       <c r="H52" s="2">
-        <f>IF(G52="facile",1,IF(G52="moyen",5,IF(G52="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I52" s="2">
@@ -2138,7 +2343,9 @@
       <c r="D53" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="2"/>
+      <c r="E53" s="2">
+        <v>36</v>
+      </c>
       <c r="F53" s="2" t="s">
         <v>23</v>
       </c>
@@ -2146,7 +2353,7 @@
         <v>43</v>
       </c>
       <c r="H53" s="2">
-        <f>IF(G53="facile",1,IF(G53="moyen",5,IF(G53="difficile",10,7.5)))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I53" s="2">

</xml_diff>